<commit_message>
LP WIP - Loans
</commit_message>
<xml_diff>
--- a/specifications/lp/Business intelligence systems - Project - Loan Portfolio Data Specification - V6.5.xlsx
+++ b/specifications/lp/Business intelligence systems - Project - Loan Portfolio Data Specification - V6.5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ShrForms\specifications\lp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C73B66C-3EAC-474C-8E61-2D4A62CC58B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A25434-9D76-486A-B8C5-D9B68ABA6192}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="804" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="804" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version Control" sheetId="2" r:id="rId1"/>
@@ -37,6 +37,9 @@
     <sheet name="LOV Embedded Int Rate Deriv" sheetId="23" state="hidden" r:id="rId22"/>
   </sheets>
   <definedNames>
+    <definedName name="pfo_count_eird">Data!$G$5</definedName>
+    <definedName name="pfo_count_erd">Data!$G$5</definedName>
+    <definedName name="pfo_count_erds">Data!$G$5</definedName>
     <definedName name="Pfo_Page_Serial">Data!$G$3</definedName>
     <definedName name="Pfo_Page_Serial_Padded_4">Data!$G$4</definedName>
     <definedName name="Pfo_Serial">Data!$G$3</definedName>
@@ -56,8 +59,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2660" uniqueCount="1641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2656" uniqueCount="1640">
   <si>
     <t>Field ID</t>
   </si>
@@ -4986,18 +5011,6 @@
     <t>Validation #6 Formula</t>
   </si>
   <si>
-    <t>12. First interest payment date must be the same as or earlier than 11. Final Capial Repayment Date</t>
-  </si>
-  <si>
-    <t>12. First interest payment date must be the same as 10. First Capital Repayment Date for Repayment Terms</t>
-  </si>
-  <si>
-    <t>12. First interest payment date must be prior to 10. First Capital Repayment Date for Repayment Terms</t>
-  </si>
-  <si>
-    <t>12. First interest payment date must be prior to 11. Final Capital Repayment Date for Repayment Terms</t>
-  </si>
-  <si>
     <t>If 1. Loan Type = "Fixed Rate Loan", "Fixed with embedded Intereat Rate Swaps", "Fixed without embedded Intererest Rate Swaps" or "Bond / Capital Market product", then 8. Reference Interest Rate must = "Fixed Rate Percentage"</t>
   </si>
   <si>
@@ -5335,6 +5348,15 @@
   </si>
   <si>
     <t>Choice(reference_interest_rate.csv,3)</t>
+  </si>
+  <si>
+    <t>12. First interest payment date must be the same as or earlier than 11. Final Capital Repayment Date</t>
+  </si>
+  <si>
+    <t>close({"closeChildren":true, "closeLabel":"Repay loan", "message":"Are you sure you want to repay this loan?", "closedMessage":"Loan has been repaid", "cantCloseMessage":"Can't mark this loan as repaid."})</t>
+  </si>
+  <si>
+    <t>Interest Rate Derivative exists but Loan type not (Fixed with embedded Interest Rate Swaps) OR(Revolving Loan / Credit Facility) OR (Variable with embedded Interest Rate Swaps)</t>
   </si>
 </sst>
 </file>
@@ -6476,6 +6498,10 @@
     <xf numFmtId="166" fontId="13" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6512,13 +6538,10 @@
     <xf numFmtId="0" fontId="32" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6527,10 +6550,9 @@
     <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="4" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Heading" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -7851,10 +7873,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="204" t="s">
+      <c r="B2" s="206" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="205"/>
+      <c r="C2" s="207"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
@@ -8441,7 +8463,7 @@
         <v>1006</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>1535</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
@@ -8455,7 +8477,7 @@
         <v>1006</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>1635</v>
+        <v>1631</v>
       </c>
     </row>
   </sheetData>
@@ -8678,9 +8700,9 @@
       <c r="A42" s="44" t="s">
         <v>998</v>
       </c>
-      <c r="B42" t="str">
+      <c r="B42">
         <f>Data!H151</f>
-        <v>No</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
@@ -8817,10 +8839,10 @@
       <c r="C72" s="74" t="s">
         <v>336</v>
       </c>
-      <c r="D72" s="212" t="s">
+      <c r="D72" s="214" t="s">
         <v>338</v>
       </c>
-      <c r="E72" s="213"/>
+      <c r="E72" s="215"/>
       <c r="F72" s="137"/>
       <c r="G72" s="137"/>
     </row>
@@ -8833,11 +8855,11 @@
         <f>Data!H167</f>
         <v>Debt Service Test (DST)</v>
       </c>
-      <c r="D73" s="214" t="str">
+      <c r="D73" s="216" t="str">
         <f>Data!H170</f>
         <v>Monthly</v>
       </c>
-      <c r="E73" s="214"/>
+      <c r="E73" s="216"/>
       <c r="F73" s="152" t="s">
         <v>1121</v>
       </c>
@@ -8864,8 +8886,8 @@
       <c r="E77" s="74" t="s">
         <v>172</v>
       </c>
-      <c r="F77" s="206"/>
-      <c r="G77" s="207"/>
+      <c r="F77" s="208"/>
+      <c r="G77" s="209"/>
     </row>
     <row r="78" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="79">
@@ -9242,15 +9264,15 @@
       <c r="C8" s="74" t="s">
         <v>1120</v>
       </c>
-      <c r="D8" s="215" t="s">
+      <c r="D8" s="217" t="s">
         <v>173</v>
       </c>
       <c r="E8" s="218"/>
-      <c r="F8" s="216"/>
-      <c r="G8" s="215" t="s">
+      <c r="F8" s="219"/>
+      <c r="G8" s="217" t="s">
         <v>174</v>
       </c>
-      <c r="H8" s="216"/>
+      <c r="H8" s="219"/>
       <c r="I8" s="74"/>
       <c r="J8" s="74"/>
     </row>
@@ -9258,15 +9280,15 @@
       <c r="C9" s="75">
         <v>1431</v>
       </c>
-      <c r="D9" s="219" t="s">
+      <c r="D9" s="220" t="s">
         <v>448</v>
       </c>
-      <c r="E9" s="219"/>
-      <c r="F9" s="219"/>
-      <c r="G9" s="217">
+      <c r="E9" s="220"/>
+      <c r="F9" s="220"/>
+      <c r="G9" s="222">
         <v>1000.1</v>
       </c>
-      <c r="H9" s="217"/>
+      <c r="H9" s="222"/>
       <c r="I9" s="78" t="s">
         <v>1121</v>
       </c>
@@ -9278,15 +9300,15 @@
       <c r="C10" s="75">
         <v>1432</v>
       </c>
-      <c r="D10" s="219" t="s">
+      <c r="D10" s="220" t="s">
         <v>457</v>
       </c>
-      <c r="E10" s="219"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="217">
+      <c r="E10" s="220"/>
+      <c r="F10" s="220"/>
+      <c r="G10" s="222">
         <v>2000.9</v>
       </c>
-      <c r="H10" s="217"/>
+      <c r="H10" s="222"/>
       <c r="I10" s="78" t="s">
         <v>1121</v>
       </c>
@@ -9308,15 +9330,15 @@
       <c r="C12" s="74" t="s">
         <v>1120</v>
       </c>
-      <c r="D12" s="215" t="s">
+      <c r="D12" s="217" t="s">
         <v>336</v>
       </c>
-      <c r="E12" s="216"/>
-      <c r="F12" s="215" t="s">
+      <c r="E12" s="219"/>
+      <c r="F12" s="217" t="s">
         <v>338</v>
       </c>
       <c r="G12" s="218"/>
-      <c r="H12" s="216"/>
+      <c r="H12" s="219"/>
       <c r="I12" s="74"/>
       <c r="J12" s="74"/>
     </row>
@@ -9324,15 +9346,15 @@
       <c r="C13" s="75">
         <v>13475</v>
       </c>
-      <c r="D13" s="219" t="s">
+      <c r="D13" s="220" t="s">
         <v>899</v>
       </c>
-      <c r="E13" s="219"/>
-      <c r="F13" s="219" t="s">
+      <c r="E13" s="220"/>
+      <c r="F13" s="220" t="s">
         <v>878</v>
       </c>
-      <c r="G13" s="219"/>
-      <c r="H13" s="219"/>
+      <c r="G13" s="220"/>
+      <c r="H13" s="220"/>
       <c r="I13" s="78" t="s">
         <v>1121</v>
       </c>
@@ -9344,15 +9366,15 @@
       <c r="C14" s="75">
         <v>13476</v>
       </c>
-      <c r="D14" s="219" t="s">
+      <c r="D14" s="220" t="s">
         <v>917</v>
       </c>
-      <c r="E14" s="219"/>
-      <c r="F14" s="219" t="s">
+      <c r="E14" s="220"/>
+      <c r="F14" s="220" t="s">
         <v>880</v>
       </c>
-      <c r="G14" s="219"/>
-      <c r="H14" s="219"/>
+      <c r="G14" s="220"/>
+      <c r="H14" s="220"/>
       <c r="I14" s="78" t="s">
         <v>1121</v>
       </c>
@@ -9559,11 +9581,11 @@
       <c r="D25" s="74" t="s">
         <v>165</v>
       </c>
-      <c r="E25" s="215" t="s">
+      <c r="E25" s="217" t="s">
         <v>332</v>
       </c>
       <c r="F25" s="218"/>
-      <c r="G25" s="216"/>
+      <c r="G25" s="219"/>
       <c r="H25" s="74" t="s">
         <v>1123</v>
       </c>
@@ -9620,15 +9642,15 @@
       <c r="C29" s="74" t="s">
         <v>1120</v>
       </c>
-      <c r="D29" s="215" t="s">
+      <c r="D29" s="217" t="s">
         <v>336</v>
       </c>
-      <c r="E29" s="216"/>
-      <c r="F29" s="215" t="s">
+      <c r="E29" s="219"/>
+      <c r="F29" s="217" t="s">
         <v>338</v>
       </c>
       <c r="G29" s="218"/>
-      <c r="H29" s="216"/>
+      <c r="H29" s="219"/>
       <c r="I29" s="80"/>
       <c r="J29" s="74"/>
     </row>
@@ -9636,15 +9658,15 @@
       <c r="C30" s="75">
         <v>13473</v>
       </c>
-      <c r="D30" s="219" t="s">
+      <c r="D30" s="220" t="s">
         <v>899</v>
       </c>
-      <c r="E30" s="219"/>
-      <c r="F30" s="219" t="s">
+      <c r="E30" s="220"/>
+      <c r="F30" s="220" t="s">
         <v>878</v>
       </c>
-      <c r="G30" s="219"/>
-      <c r="H30" s="219"/>
+      <c r="G30" s="220"/>
+      <c r="H30" s="220"/>
       <c r="I30" s="78" t="s">
         <v>1121</v>
       </c>
@@ -9656,15 +9678,15 @@
       <c r="C31" s="75">
         <v>13474</v>
       </c>
-      <c r="D31" s="219" t="s">
+      <c r="D31" s="220" t="s">
         <v>921</v>
       </c>
-      <c r="E31" s="219"/>
-      <c r="F31" s="219" t="s">
+      <c r="E31" s="220"/>
+      <c r="F31" s="220" t="s">
         <v>880</v>
       </c>
-      <c r="G31" s="219"/>
-      <c r="H31" s="219"/>
+      <c r="G31" s="220"/>
+      <c r="H31" s="220"/>
       <c r="I31" s="78" t="s">
         <v>1121</v>
       </c>
@@ -9680,14 +9702,14 @@
       <c r="C33" s="74" t="s">
         <v>1120</v>
       </c>
-      <c r="D33" s="215" t="s">
+      <c r="D33" s="217" t="s">
         <v>356</v>
       </c>
-      <c r="E33" s="216"/>
-      <c r="F33" s="215" t="s">
+      <c r="E33" s="219"/>
+      <c r="F33" s="217" t="s">
         <v>171</v>
       </c>
-      <c r="G33" s="216"/>
+      <c r="G33" s="219"/>
       <c r="H33" s="81" t="s">
         <v>172</v>
       </c>
@@ -9698,14 +9720,14 @@
       <c r="C34" s="75">
         <v>1454</v>
       </c>
-      <c r="D34" s="219" t="s">
+      <c r="D34" s="220" t="s">
         <v>1140</v>
       </c>
-      <c r="E34" s="219"/>
-      <c r="F34" s="220">
+      <c r="E34" s="220"/>
+      <c r="F34" s="221">
         <v>43133</v>
       </c>
-      <c r="G34" s="220"/>
+      <c r="G34" s="221"/>
       <c r="H34" s="84">
         <v>43134</v>
       </c>
@@ -9720,14 +9742,14 @@
       <c r="C35" s="75">
         <v>1455</v>
       </c>
-      <c r="D35" s="219" t="s">
+      <c r="D35" s="220" t="s">
         <v>1140</v>
       </c>
-      <c r="E35" s="219"/>
-      <c r="F35" s="220">
+      <c r="E35" s="220"/>
+      <c r="F35" s="221">
         <v>43132</v>
       </c>
-      <c r="G35" s="220"/>
+      <c r="G35" s="221"/>
       <c r="H35" s="84">
         <v>43159</v>
       </c>
@@ -9743,6 +9765,24 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="D33:E33"/>
     <mergeCell ref="E25:G25"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="F30:H30"/>
@@ -9750,24 +9790,6 @@
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14297,16 +14319,16 @@
         <v>345</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>1542</v>
+        <v>1538</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>346</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>1543</v>
+        <v>1539</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>1544</v>
+        <v>1540</v>
       </c>
       <c r="F1" s="31" t="s">
         <v>146</v>
@@ -14559,18 +14581,18 @@
     </row>
     <row r="2" spans="1:251" x14ac:dyDescent="0.2">
       <c r="A2" s="88" t="s">
-        <v>1565</v>
+        <v>1561</v>
       </c>
       <c r="B2" s="88"/>
       <c r="C2" s="88" t="s">
-        <v>1565</v>
+        <v>1561</v>
       </c>
       <c r="D2" s="88"/>
       <c r="E2" s="88" t="s">
-        <v>1566</v>
+        <v>1562</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>1565</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="3" spans="1:251" x14ac:dyDescent="0.2">
@@ -14591,18 +14613,18 @@
     </row>
     <row r="4" spans="1:251" x14ac:dyDescent="0.2">
       <c r="A4" s="88" t="s">
-        <v>1567</v>
+        <v>1563</v>
       </c>
       <c r="B4" s="88"/>
       <c r="C4" s="88" t="s">
-        <v>1567</v>
+        <v>1563</v>
       </c>
       <c r="D4" s="88"/>
       <c r="E4" s="88" t="s">
-        <v>1568</v>
+        <v>1564</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>1567</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="5" spans="1:251" x14ac:dyDescent="0.2">
@@ -14611,14 +14633,14 @@
       </c>
       <c r="B5" s="39"/>
       <c r="C5" s="33" t="s">
-        <v>1545</v>
+        <v>1541</v>
       </c>
       <c r="D5" s="33"/>
       <c r="E5" s="33" t="s">
-        <v>1545</v>
+        <v>1541</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>1548</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="6" spans="1:251" x14ac:dyDescent="0.2">
@@ -14627,14 +14649,14 @@
       </c>
       <c r="B6" s="39"/>
       <c r="C6" t="s">
-        <v>1550</v>
+        <v>1546</v>
       </c>
       <c r="D6" s="33"/>
       <c r="E6" t="s">
-        <v>1550</v>
+        <v>1546</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>1549</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="7" spans="1:251" x14ac:dyDescent="0.2">
@@ -14659,11 +14681,11 @@
       </c>
       <c r="B8" s="39"/>
       <c r="C8" s="33" t="s">
-        <v>1551</v>
+        <v>1547</v>
       </c>
       <c r="D8" s="33"/>
       <c r="E8" s="33" t="s">
-        <v>1551</v>
+        <v>1547</v>
       </c>
       <c r="F8" s="34" t="s">
         <v>1007</v>
@@ -14707,11 +14729,11 @@
       </c>
       <c r="B11" s="39"/>
       <c r="C11" s="88" t="s">
-        <v>1580</v>
+        <v>1576</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="88" t="s">
-        <v>1580</v>
+        <v>1576</v>
       </c>
       <c r="F11" s="88" t="s">
         <v>1010</v>
@@ -14723,10 +14745,10 @@
       </c>
       <c r="B12" s="39"/>
       <c r="C12" s="33" t="s">
-        <v>1582</v>
+        <v>1578</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>1582</v>
+        <v>1578</v>
       </c>
       <c r="F12" s="39" t="s">
         <v>1017</v>
@@ -15335,9 +15357,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q144" sqref="Q144"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O136" sqref="O136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15376,14 +15398,14 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B2" s="156" t="s">
-        <v>1536</v>
+        <v>1532</v>
       </c>
       <c r="C2" s="157"/>
       <c r="D2" s="155"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B3" s="158" t="s">
-        <v>1537</v>
+        <v>1533</v>
       </c>
       <c r="C3" s="158"/>
       <c r="D3" s="159"/>
@@ -15393,18 +15415,21 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B4" s="158" t="s">
-        <v>1538</v>
+        <v>1534</v>
       </c>
       <c r="C4" s="158"/>
       <c r="D4" s="160"/>
       <c r="G4" s="186" t="s">
-        <v>1592</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B5" s="154"/>
       <c r="C5" s="154"/>
       <c r="D5" s="155"/>
+      <c r="G5" s="186">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B6" s="154"/>
@@ -15482,10 +15507,10 @@
         <v>1524</v>
       </c>
       <c r="W8" s="11" t="s">
-        <v>1539</v>
+        <v>1535</v>
       </c>
       <c r="X8" s="11" t="s">
-        <v>1540</v>
+        <v>1536</v>
       </c>
       <c r="Y8" s="11" t="s">
         <v>138</v>
@@ -15555,7 +15580,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="10" t="s">
-        <v>1633</v>
+        <v>1629</v>
       </c>
       <c r="O10" s="101"/>
       <c r="P10" s="10"/>
@@ -15599,7 +15624,7 @@
       </c>
       <c r="I11" s="106"/>
       <c r="J11" s="100" t="s">
-        <v>1587</v>
+        <v>1583</v>
       </c>
       <c r="K11" s="107" t="s">
         <v>131</v>
@@ -15689,14 +15714,12 @@
         <v>Submission.LPR005</v>
       </c>
       <c r="D13" s="108" t="s">
-        <v>1572</v>
+        <v>1568</v>
       </c>
       <c r="E13" s="107" t="s">
         <v>128</v>
       </c>
-      <c r="F13" s="107" t="s">
-        <v>1258</v>
-      </c>
+      <c r="F13" s="107"/>
       <c r="G13" s="108"/>
       <c r="H13" s="105">
         <v>44286</v>
@@ -15717,10 +15740,7 @@
       <c r="T13" s="108"/>
       <c r="U13" s="101"/>
       <c r="V13" s="108"/>
-      <c r="W13" s="194" t="b">
-        <f>H190 = "Annual"</f>
-        <v>1</v>
-      </c>
+      <c r="W13" s="194"/>
       <c r="X13" s="108"/>
       <c r="Y13" s="108" t="s">
         <v>231</v>
@@ -15739,7 +15759,7 @@
         <v>Submission.LPR005a</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>1572</v>
+        <v>1568</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>128</v>
@@ -15767,10 +15787,7 @@
       <c r="T14" s="10"/>
       <c r="U14" s="101"/>
       <c r="V14" s="10"/>
-      <c r="W14" s="118" t="b">
-        <f>H190 = "In-Year"</f>
-        <v>0</v>
-      </c>
+      <c r="W14" s="118"/>
       <c r="X14" s="10"/>
       <c r="Y14" s="27" t="s">
         <v>231</v>
@@ -16106,7 +16123,7 @@
     <row r="22" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15"/>
       <c r="B22" s="177" t="s">
-        <v>1563</v>
+        <v>1559</v>
       </c>
       <c r="C22" s="177" t="str">
         <f>"Submission." &amp; B22</f>
@@ -16116,7 +16133,7 @@
         <v>1008</v>
       </c>
       <c r="E22" s="179" t="s">
-        <v>1564</v>
+        <v>1560</v>
       </c>
       <c r="F22" s="181"/>
       <c r="G22" s="181"/>
@@ -16143,7 +16160,7 @@
     <row r="23" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
       <c r="B23" s="177" t="s">
-        <v>1554</v>
+        <v>1550</v>
       </c>
       <c r="C23" s="177" t="str">
         <f t="shared" ref="C23" si="1">"Submission." &amp; B23</f>
@@ -16153,7 +16170,7 @@
         <v>892</v>
       </c>
       <c r="E23" s="179" t="s">
-        <v>1558</v>
+        <v>1554</v>
       </c>
       <c r="F23" s="181"/>
       <c r="G23" s="181"/>
@@ -16180,17 +16197,17 @@
     <row r="24" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
       <c r="B24" s="177" t="s">
-        <v>1546</v>
+        <v>1542</v>
       </c>
       <c r="C24" s="177" t="str">
         <f t="shared" si="0"/>
         <v>Submission.LPR100</v>
       </c>
       <c r="D24" s="178" t="s">
-        <v>1556</v>
+        <v>1552</v>
       </c>
       <c r="E24" s="180" t="s">
-        <v>1547</v>
+        <v>1543</v>
       </c>
       <c r="F24" s="181"/>
       <c r="G24" s="181"/>
@@ -16217,17 +16234,17 @@
     <row r="25" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
       <c r="B25" s="177" t="s">
-        <v>1552</v>
+        <v>1548</v>
       </c>
       <c r="C25" s="177" t="str">
         <f t="shared" ref="C25" si="2">"Submission." &amp; B25</f>
         <v>Submission.LPR101</v>
       </c>
       <c r="D25" s="178" t="s">
-        <v>1555</v>
+        <v>1551</v>
       </c>
       <c r="E25" s="179" t="s">
-        <v>1557</v>
+        <v>1553</v>
       </c>
       <c r="F25" s="181"/>
       <c r="G25" s="181"/>
@@ -16502,7 +16519,7 @@
         <v>1</v>
       </c>
       <c r="N31" s="10" t="s">
-        <v>1625</v>
+        <v>1621</v>
       </c>
       <c r="O31" s="101"/>
       <c r="P31" s="10"/>
@@ -16725,7 +16742,7 @@
         <v>IGFLend.LPIGF009</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>1573</v>
+        <v>1569</v>
       </c>
       <c r="E36" s="9" t="s">
         <v>128</v>
@@ -16771,7 +16788,7 @@
         <v>IGFLend.LPIGF010</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>1574</v>
+        <v>1570</v>
       </c>
       <c r="E37" s="9" t="s">
         <v>128</v>
@@ -17711,7 +17728,7 @@
     <row r="57" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A57" s="15"/>
       <c r="B57" s="107" t="s">
-        <v>1553</v>
+        <v>1549</v>
       </c>
       <c r="C57" s="118" t="str">
         <f t="shared" si="4"/>
@@ -17880,7 +17897,7 @@
         <v>1</v>
       </c>
       <c r="N60" s="10" t="s">
-        <v>1624</v>
+        <v>1620</v>
       </c>
       <c r="O60" s="101"/>
       <c r="P60" s="10"/>
@@ -18103,7 +18120,7 @@
         <v>IGFBorrow.LPIGF033</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>1573</v>
+        <v>1569</v>
       </c>
       <c r="E65" s="9" t="s">
         <v>128</v>
@@ -18149,7 +18166,7 @@
         <v>IGFBorrow.LPIGF034</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>1575</v>
+        <v>1571</v>
       </c>
       <c r="E66" s="9" t="s">
         <v>128</v>
@@ -19282,7 +19299,7 @@
     </row>
     <row r="90" spans="1:26" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B90" s="23" t="s">
-        <v>1621</v>
+        <v>1617</v>
       </c>
       <c r="C90" s="118" t="str">
         <f t="shared" si="5"/>
@@ -19666,7 +19683,7 @@
         <v>183</v>
       </c>
       <c r="E98" s="23" t="s">
-        <v>1622</v>
+        <v>1618</v>
       </c>
       <c r="F98" s="17"/>
       <c r="G98" s="17"/>
@@ -19703,7 +19720,7 @@
     <row r="99" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="15"/>
       <c r="B99" s="177" t="s">
-        <v>1560</v>
+        <v>1556</v>
       </c>
       <c r="C99" s="184" t="str">
         <f>"ISDA." &amp; B99</f>
@@ -19713,7 +19730,7 @@
         <v>1007</v>
       </c>
       <c r="E99" s="180" t="s">
-        <v>1562</v>
+        <v>1558</v>
       </c>
       <c r="F99" s="181"/>
       <c r="G99" s="181"/>
@@ -19873,7 +19890,7 @@
         <v>336</v>
       </c>
       <c r="E103" s="23" t="s">
-        <v>1559</v>
+        <v>1555</v>
       </c>
       <c r="F103" s="17"/>
       <c r="G103" s="17"/>
@@ -20230,7 +20247,7 @@
         <v>Facility.LPF001</v>
       </c>
       <c r="D111" s="16" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
       <c r="E111" s="23" t="s">
         <v>1347</v>
@@ -20242,7 +20259,7 @@
       </c>
       <c r="I111" s="104"/>
       <c r="J111" s="103" t="s">
-        <v>1576</v>
+        <v>1572</v>
       </c>
       <c r="K111" s="9" t="s">
         <v>129</v>
@@ -20327,7 +20344,7 @@
         <v>342</v>
       </c>
       <c r="E113" s="23" t="s">
-        <v>1620</v>
+        <v>1616</v>
       </c>
       <c r="F113" s="17"/>
       <c r="G113" s="17"/>
@@ -20389,7 +20406,7 @@
         <v>DMOBOS0002</v>
       </c>
       <c r="J114" s="119" t="s">
-        <v>1634</v>
+        <v>1630</v>
       </c>
       <c r="K114" s="107"/>
       <c r="L114" s="108"/>
@@ -20470,7 +20487,7 @@
         <v>1361</v>
       </c>
       <c r="E116" s="23" t="s">
-        <v>1619</v>
+        <v>1615</v>
       </c>
       <c r="F116" s="17"/>
       <c r="G116" s="17"/>
@@ -20870,7 +20887,7 @@
         <v>404</v>
       </c>
       <c r="E124" s="23" t="s">
-        <v>1561</v>
+        <v>1557</v>
       </c>
       <c r="F124" s="17"/>
       <c r="G124" s="17"/>
@@ -21236,7 +21253,7 @@
     <row r="132" spans="1:27" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="15"/>
       <c r="B132" s="177" t="s">
-        <v>1560</v>
+        <v>1556</v>
       </c>
       <c r="C132" s="184" t="str">
         <f>"Facility." &amp; B132</f>
@@ -21246,7 +21263,7 @@
         <v>1042</v>
       </c>
       <c r="E132" s="179" t="s">
-        <v>1579</v>
+        <v>1575</v>
       </c>
       <c r="F132" s="181"/>
       <c r="G132" s="181"/>
@@ -21273,7 +21290,7 @@
     <row r="133" spans="1:27" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="15"/>
       <c r="B133" s="177" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="C133" s="184" t="str">
         <f>"Facility." &amp; B133</f>
@@ -21283,7 +21300,7 @@
         <v>1010</v>
       </c>
       <c r="E133" s="179" t="s">
-        <v>1591</v>
+        <v>1587</v>
       </c>
       <c r="F133" s="181"/>
       <c r="G133" s="181"/>
@@ -21397,7 +21414,7 @@
         <v>162</v>
       </c>
       <c r="E136" s="23" t="s">
-        <v>1637</v>
+        <v>1633</v>
       </c>
       <c r="F136" s="17"/>
       <c r="G136" s="17"/>
@@ -21412,12 +21429,20 @@
       <c r="L136" s="10" t="s">
         <v>1261</v>
       </c>
-      <c r="M136" s="116"/>
+      <c r="M136" s="116" t="b" cm="1">
+        <f t="array" ref="M136">IF(OR(H136="FWEIRS",H136="VWES"),pfo_count_eird&gt;0,TRUE)</f>
+        <v>1</v>
+      </c>
       <c r="N136" s="10" t="s">
         <v>1522</v>
       </c>
-      <c r="O136" s="101"/>
-      <c r="P136" s="10"/>
+      <c r="O136" s="101" t="b" cm="1">
+        <f t="array" ref="O136">IF(pfo_count_eird &gt; 0,OR(H136="FWEIRS",H136="REVLNF",H136="VWES"), TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="P136" s="10" t="s">
+        <v>1639</v>
+      </c>
       <c r="Q136" s="101"/>
       <c r="R136" s="10"/>
       <c r="S136" s="101"/>
@@ -21492,7 +21517,7 @@
         <v>163</v>
       </c>
       <c r="E138" s="23" t="s">
-        <v>1638</v>
+        <v>1634</v>
       </c>
       <c r="F138" s="17"/>
       <c r="G138" s="17"/>
@@ -21755,7 +21780,7 @@
         <v>166</v>
       </c>
       <c r="E143" s="23" t="s">
-        <v>1639</v>
+        <v>1635</v>
       </c>
       <c r="F143" s="17"/>
       <c r="G143" s="17"/>
@@ -21801,7 +21826,7 @@
         <v>167</v>
       </c>
       <c r="E144" s="23" t="s">
-        <v>1640</v>
+        <v>1636</v>
       </c>
       <c r="F144" s="17"/>
       <c r="G144" s="17"/>
@@ -21810,7 +21835,7 @@
       </c>
       <c r="I144" s="104"/>
       <c r="J144" s="100" t="s">
-        <v>1532</v>
+        <v>1528</v>
       </c>
       <c r="K144" s="9" t="s">
         <v>129</v>
@@ -21823,25 +21848,28 @@
         <v>1</v>
       </c>
       <c r="N144" s="10" t="s">
-        <v>1530</v>
+        <v>1526</v>
       </c>
       <c r="O144" s="101" t="b">
         <f>IF(H136="FIXIF",H144=4, TRUE)</f>
         <v>1</v>
       </c>
       <c r="P144" s="10" t="s">
-        <v>1531</v>
+        <v>1527</v>
       </c>
       <c r="Q144" s="101" t="b">
         <f>IF(H144=3, OR(H136="FIXED",H136="FWEIRS",H136="FNEIRS", H136="BNDCAP"), TRUE)</f>
         <v>0</v>
       </c>
       <c r="R144" s="10" t="s">
-        <v>1533</v>
-      </c>
-      <c r="S144" s="101"/>
+        <v>1529</v>
+      </c>
+      <c r="S144" s="101" t="b">
+        <f>IF(H144=4,H136="FIXIF",TRUE)</f>
+        <v>1</v>
+      </c>
       <c r="T144" s="10" t="s">
-        <v>1534</v>
+        <v>1530</v>
       </c>
       <c r="U144" s="101"/>
       <c r="V144" s="10"/>
@@ -21894,7 +21922,7 @@
       <c r="T145" s="10"/>
       <c r="U145" s="101"/>
       <c r="V145" s="10"/>
-      <c r="W145" s="222" t="b">
+      <c r="W145" s="205" t="b">
         <f>AND(H136&lt;&gt;"FIXIF",H136&lt;&gt;"BNDCAP",H136&lt;&gt;"FIXED", H136&lt;&gt;"FWEIRS",H136&lt;&gt;"FNEIRS")</f>
         <v>1</v>
       </c>
@@ -21906,7 +21934,7 @@
     </row>
     <row r="146" spans="2:27" ht="116.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B146" s="23" t="s">
-        <v>1593</v>
+        <v>1589</v>
       </c>
       <c r="C146" s="118" t="str">
         <f t="shared" si="8"/>
@@ -21944,7 +21972,7 @@
       <c r="T146" s="10"/>
       <c r="U146" s="101"/>
       <c r="V146" s="10"/>
-      <c r="W146" s="221" t="b">
+      <c r="W146" s="204" t="b">
         <f>NOT(AND(H136&lt;&gt;"FIXIF",H136&lt;&gt;"BNDCAP",H136&lt;&gt;"FIXED", H136&lt;&gt;"FWEIRS",H136&lt;&gt;"FNEIRS"))</f>
         <v>0</v>
       </c>
@@ -22034,8 +22062,8 @@
         <v>1463</v>
       </c>
       <c r="O148" s="122" t="b">
-        <f>AND(ABS(H148-I13)&lt;=H200,ABS(I13-H148)&lt;=H200)</f>
-        <v>0</v>
+        <f>AND(H148&gt;=H206, H148&lt;=H207)</f>
+        <v>1</v>
       </c>
       <c r="P148" s="10" t="s">
         <v>1466</v>
@@ -22093,8 +22121,8 @@
         <v>1465</v>
       </c>
       <c r="O149" s="122" t="b">
-        <f>AND(ABS(JH149-I13)&lt;=H201,ABS(I13-H149)&lt;=H200)</f>
-        <v>0</v>
+        <f>AND(H149&gt;=H206,H149&lt;=H207)</f>
+        <v>1</v>
       </c>
       <c r="P149" s="10" t="s">
         <v>1467</v>
@@ -22151,29 +22179,14 @@
         <v>1</v>
       </c>
       <c r="P150" s="10" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Q150" s="101" t="b">
-        <f>OR(OR(H143="Interest only - Bullet repayment at end of term from cashflow",H143="Interest only - Bullet repayment at end of term from refinancing",H143="Interest only then capital and interest",H143="Interest only until fully drawn",H143="Interest only followed by structured capital repayments",H143="Repayable on demand",H143="Converted to loan",H143="Subject to annual renewal"),AND(OR(H143="Fully Amortising",H143="Payment start date deferred then fully amortising", H143="Payment start date deferred-bullet repayment of interest and capital at maturity",H143="Interest &amp; capital then bullet repayment from cashflow or refinancing"),H150=H148))</f>
-        <v>0</v>
-      </c>
-      <c r="R150" s="10" t="s">
-        <v>1527</v>
-      </c>
-      <c r="S150" s="101" t="b">
-        <f>OR(OR(H143="Fully Amortising",H143="Payment start date deferred then fully amortising", H143="Payment start date deferred-bullet repayment of interest and capital at maturity",H143="Interest &amp; capital then bullet repayment from cashflow or refinancing",H143="Interest only - Bullet repayment at end of term from cashflow",H143="Interest only - Bullet repayment at end of term from refinancing", H143="Repayable on demand",H143="Converted to loan",H143="Subject to annual renewal"),AND(OR(H143="Interest only then capital and interest",H143="Interest only until fully drawn",H143="Interest only followed by structured capital repayments",),J150&lt;J148))</f>
-        <v>1</v>
-      </c>
-      <c r="T150" s="10" t="s">
-        <v>1528</v>
-      </c>
-      <c r="U150" s="101" t="b">
-        <f>OR(OR(H143="Fully Amortising",H143="Payment start date deferred then fully amortising", H143="Payment start date deferred-bullet repayment of interest and capital at maturity",H143="Interest &amp; capital then bullet repayment from cashflow or refinancing", H143="Interest only then capital and interest", H143="Interest only followed by structured capital repayments",H143="Repayable on demand",H143="Converted to loan",H143="Subject to annual renewal"),AND(OR(H143="Interest only - Bullet repayment at end of term from cashflow",H143="Interest only - Bullet repayment at end of term from refinancing",H143="Interest only until fully drawn",),L150&lt;L149))</f>
-        <v>1</v>
-      </c>
-      <c r="V150" s="10" t="s">
-        <v>1529</v>
-      </c>
+        <v>1637</v>
+      </c>
+      <c r="Q150" s="101"/>
+      <c r="R150" s="10"/>
+      <c r="S150" s="101"/>
+      <c r="T150" s="10"/>
+      <c r="U150" s="101"/>
+      <c r="V150" s="10"/>
       <c r="W150" s="118" t="b">
         <f>AND( H144&lt;&gt;4,H144&lt;&gt;5)</f>
         <v>1</v>
@@ -22202,8 +22215,8 @@
       </c>
       <c r="F151" s="17"/>
       <c r="G151" s="17"/>
-      <c r="H151" s="103" t="s">
-        <v>934</v>
+      <c r="H151" s="103">
+        <v>2</v>
       </c>
       <c r="I151" s="104"/>
       <c r="J151" s="100"/>
@@ -22279,7 +22292,7 @@
       <c r="V152" s="61"/>
       <c r="W152" s="118" t="b">
         <f>H151=2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X152" s="10"/>
       <c r="Y152" s="16" t="s">
@@ -22327,7 +22340,7 @@
       <c r="V153" s="61"/>
       <c r="W153" s="118" t="b">
         <f>H151=2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X153" s="10"/>
       <c r="Y153" s="16" t="s">
@@ -22350,7 +22363,7 @@
         <v>968</v>
       </c>
       <c r="E154" s="23" t="s">
-        <v>1578</v>
+        <v>1574</v>
       </c>
       <c r="F154" s="17"/>
       <c r="G154" s="17"/>
@@ -22774,8 +22787,8 @@
       <c r="D163" s="16" t="s">
         <v>1000</v>
       </c>
-      <c r="E163" s="23" t="s">
-        <v>1375</v>
+      <c r="E163" s="178" t="s">
+        <v>1638</v>
       </c>
       <c r="F163" s="17"/>
       <c r="G163" s="17"/>
@@ -22815,17 +22828,17 @@
     <row r="164" spans="1:27" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="15"/>
       <c r="B164" s="177" t="s">
-        <v>1583</v>
+        <v>1579</v>
       </c>
       <c r="C164" s="118" t="str">
         <f t="shared" si="8"/>
         <v>Loan.LPL100</v>
       </c>
       <c r="D164" s="178" t="s">
-        <v>1584</v>
+        <v>1580</v>
       </c>
       <c r="E164" s="179" t="s">
-        <v>1585</v>
+        <v>1581</v>
       </c>
       <c r="F164" s="181"/>
       <c r="G164" s="181"/>
@@ -22852,17 +22865,17 @@
     <row r="165" spans="1:27" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="15"/>
       <c r="B165" s="177" t="s">
-        <v>1588</v>
+        <v>1584</v>
       </c>
       <c r="C165" s="118" t="str">
         <f t="shared" si="8"/>
         <v>Loan.LPL101</v>
       </c>
       <c r="D165" s="178" t="s">
-        <v>1589</v>
+        <v>1585</v>
       </c>
       <c r="E165" s="179" t="s">
-        <v>1590</v>
+        <v>1586</v>
       </c>
       <c r="F165" s="181"/>
       <c r="G165" s="181"/>
@@ -22947,7 +22960,7 @@
         <v>336</v>
       </c>
       <c r="E167" s="23" t="s">
-        <v>1559</v>
+        <v>1555</v>
       </c>
       <c r="F167" s="17"/>
       <c r="G167" s="17"/>
@@ -23294,7 +23307,7 @@
         <v>1508</v>
       </c>
       <c r="E175" s="23" t="s">
-        <v>1636</v>
+        <v>1632</v>
       </c>
       <c r="F175" s="17"/>
       <c r="G175" s="17"/>
@@ -23357,7 +23370,7 @@
         <v>1</v>
       </c>
       <c r="N176" s="10" t="s">
-        <v>1623</v>
+        <v>1619</v>
       </c>
       <c r="O176" s="101"/>
       <c r="P176" s="10"/>
@@ -23561,7 +23574,7 @@
     </row>
     <row r="181" spans="1:26" s="18" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B181" s="23" t="s">
-        <v>1586</v>
+        <v>1582</v>
       </c>
       <c r="C181" s="118" t="str">
         <f t="shared" si="10"/>
@@ -23774,13 +23787,13 @@
         <v>395</v>
       </c>
       <c r="C186" s="63" t="s">
-        <v>1569</v>
+        <v>1565</v>
       </c>
       <c r="D186" s="125" t="s">
-        <v>1570</v>
+        <v>1566</v>
       </c>
       <c r="E186" s="23" t="s">
-        <v>1571</v>
+        <v>1567</v>
       </c>
       <c r="F186" s="23"/>
       <c r="G186" s="23"/>
@@ -23833,7 +23846,7 @@
     </row>
     <row r="188" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B188" s="128" t="s">
-        <v>1597</v>
+        <v>1593</v>
       </c>
       <c r="C188" s="129" t="s">
         <v>1401</v>
@@ -23870,7 +23883,7 @@
     </row>
     <row r="189" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B189" s="128" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="C189" s="129" t="s">
         <v>1405</v>
@@ -23907,7 +23920,7 @@
     </row>
     <row r="190" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B190" s="128" t="s">
-        <v>1599</v>
+        <v>1595</v>
       </c>
       <c r="C190" s="129" t="s">
         <v>1409</v>
@@ -23944,7 +23957,7 @@
     </row>
     <row r="191" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B191" s="128" t="s">
-        <v>1600</v>
+        <v>1596</v>
       </c>
       <c r="C191" s="129" t="s">
         <v>1410</v>
@@ -23981,7 +23994,7 @@
     </row>
     <row r="192" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B192" s="128" t="s">
-        <v>1601</v>
+        <v>1597</v>
       </c>
       <c r="C192" s="129" t="s">
         <v>1413</v>
@@ -24018,7 +24031,7 @@
     </row>
     <row r="193" spans="2:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B193" s="128" t="s">
-        <v>1602</v>
+        <v>1598</v>
       </c>
       <c r="C193" s="129" t="s">
         <v>1415</v>
@@ -24055,16 +24068,16 @@
     </row>
     <row r="194" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B194" s="128" t="s">
-        <v>1629</v>
+        <v>1625</v>
       </c>
       <c r="C194" s="129" t="s">
-        <v>1631</v>
+        <v>1627</v>
       </c>
       <c r="D194" s="129" t="s">
-        <v>1626</v>
+        <v>1622</v>
       </c>
       <c r="E194" s="128" t="s">
-        <v>1627</v>
+        <v>1623</v>
       </c>
       <c r="F194" s="128"/>
       <c r="G194" s="129"/>
@@ -24094,13 +24107,13 @@
     </row>
     <row r="195" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B195" s="128" t="s">
-        <v>1630</v>
+        <v>1626</v>
       </c>
       <c r="C195" s="129" t="s">
-        <v>1632</v>
+        <v>1628</v>
       </c>
       <c r="D195" s="129" t="s">
-        <v>1628</v>
+        <v>1624</v>
       </c>
       <c r="E195" s="128" t="s">
         <v>1421</v>
@@ -24133,7 +24146,7 @@
     </row>
     <row r="196" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B196" s="128" t="s">
-        <v>1603</v>
+        <v>1599</v>
       </c>
       <c r="C196" s="129" t="s">
         <v>1419</v>
@@ -24170,7 +24183,7 @@
     </row>
     <row r="197" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B197" s="128" t="s">
-        <v>1604</v>
+        <v>1600</v>
       </c>
       <c r="C197" s="129" t="s">
         <v>1422</v>
@@ -24207,7 +24220,7 @@
     </row>
     <row r="198" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B198" s="128" t="s">
-        <v>1605</v>
+        <v>1601</v>
       </c>
       <c r="C198" s="129" t="s">
         <v>1424</v>
@@ -24244,7 +24257,7 @@
     </row>
     <row r="199" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B199" s="128" t="s">
-        <v>1606</v>
+        <v>1602</v>
       </c>
       <c r="C199" s="129" t="s">
         <v>1426</v>
@@ -24281,7 +24294,7 @@
     </row>
     <row r="200" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B200" s="128" t="s">
-        <v>1607</v>
+        <v>1603</v>
       </c>
       <c r="C200" s="129" t="s">
         <v>1428</v>
@@ -24317,7 +24330,7 @@
     </row>
     <row r="201" spans="2:26" ht="318.75" x14ac:dyDescent="0.2">
       <c r="B201" s="128" t="s">
-        <v>1608</v>
+        <v>1604</v>
       </c>
       <c r="C201" s="129" t="s">
         <v>1430</v>
@@ -24352,7 +24365,7 @@
     </row>
     <row r="202" spans="2:26" ht="409.5" x14ac:dyDescent="0.2">
       <c r="B202" s="128" t="s">
-        <v>1609</v>
+        <v>1605</v>
       </c>
       <c r="C202" s="129" t="s">
         <v>1434</v>
@@ -24387,7 +24400,7 @@
     </row>
     <row r="203" spans="2:26" ht="357" x14ac:dyDescent="0.2">
       <c r="B203" s="128" t="s">
-        <v>1610</v>
+        <v>1606</v>
       </c>
       <c r="C203" s="129" t="s">
         <v>1436</v>
@@ -24422,7 +24435,7 @@
     </row>
     <row r="204" spans="2:26" ht="229.5" x14ac:dyDescent="0.2">
       <c r="B204" s="128" t="s">
-        <v>1611</v>
+        <v>1607</v>
       </c>
       <c r="C204" s="129" t="s">
         <v>1439</v>
@@ -24457,13 +24470,13 @@
     </row>
     <row r="205" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B205" s="165" t="s">
-        <v>1612</v>
+        <v>1608</v>
       </c>
       <c r="C205" s="187" t="s">
-        <v>1594</v>
+        <v>1590</v>
       </c>
       <c r="D205" s="187" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="E205" s="128" t="s">
         <v>1407</v>
@@ -24471,7 +24484,7 @@
       <c r="F205" s="164"/>
       <c r="G205" s="187"/>
       <c r="H205" s="188" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="I205" s="188"/>
       <c r="J205" s="188"/>
@@ -24492,13 +24505,13 @@
     </row>
     <row r="206" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B206" s="165" t="s">
-        <v>1613</v>
+        <v>1609</v>
       </c>
       <c r="C206" s="187" t="s">
-        <v>1614</v>
+        <v>1610</v>
       </c>
       <c r="D206" s="187" t="s">
-        <v>1615</v>
+        <v>1611</v>
       </c>
       <c r="E206" s="164" t="s">
         <v>1412</v>
@@ -24527,13 +24540,13 @@
     </row>
     <row r="207" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B207" s="165" t="s">
-        <v>1618</v>
+        <v>1614</v>
       </c>
       <c r="C207" s="187" t="s">
-        <v>1616</v>
+        <v>1612</v>
       </c>
       <c r="D207" s="187" t="s">
-        <v>1617</v>
+        <v>1613</v>
       </c>
       <c r="E207" s="164" t="s">
         <v>1412</v>
@@ -24562,7 +24575,7 @@
     </row>
     <row r="208" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B208" s="165" t="s">
-        <v>1541</v>
+        <v>1537</v>
       </c>
     </row>
   </sheetData>
@@ -24892,25 +24905,25 @@
       <c r="B41" s="44" t="s">
         <v>892</v>
       </c>
-      <c r="C41" s="208"/>
-      <c r="D41" s="208"/>
-      <c r="E41" s="208"/>
+      <c r="C41" s="210"/>
+      <c r="D41" s="210"/>
+      <c r="E41" s="210"/>
     </row>
     <row r="42" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="44"/>
       <c r="B42" s="80" t="s">
         <v>1120</v>
       </c>
-      <c r="C42" s="206" t="s">
+      <c r="C42" s="208" t="s">
         <v>173</v>
       </c>
-      <c r="D42" s="209"/>
-      <c r="E42" s="207"/>
-      <c r="F42" s="206" t="s">
+      <c r="D42" s="211"/>
+      <c r="E42" s="209"/>
+      <c r="F42" s="208" t="s">
         <v>174</v>
       </c>
-      <c r="G42" s="209"/>
-      <c r="H42" s="207"/>
+      <c r="G42" s="211"/>
+      <c r="H42" s="209"/>
       <c r="I42" s="80"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -24919,18 +24932,18 @@
         <f>Data!I83</f>
         <v>1</v>
       </c>
-      <c r="C43" s="210" t="str">
+      <c r="C43" s="212" t="str">
         <f>Data!H84</f>
         <v>Clydesdale Bank plc</v>
       </c>
-      <c r="D43" s="210"/>
-      <c r="E43" s="210"/>
-      <c r="F43" s="211">
+      <c r="D43" s="212"/>
+      <c r="E43" s="212"/>
+      <c r="F43" s="213">
         <f>Data!H85</f>
         <v>10000</v>
       </c>
-      <c r="G43" s="211"/>
-      <c r="H43" s="211"/>
+      <c r="G43" s="213"/>
+      <c r="H43" s="213"/>
       <c r="I43" t="s">
         <v>1143</v>
       </c>
@@ -24960,10 +24973,10 @@
       <c r="B48" s="80" t="s">
         <v>1120</v>
       </c>
-      <c r="C48" s="206" t="s">
+      <c r="C48" s="208" t="s">
         <v>1126</v>
       </c>
-      <c r="D48" s="207"/>
+      <c r="D48" s="209"/>
       <c r="E48" s="80" t="s">
         <v>1127</v>
       </c>
@@ -25012,8 +25025,8 @@
       <c r="B50" s="80" t="s">
         <v>1137</v>
       </c>
-      <c r="C50" s="206"/>
-      <c r="D50" s="207"/>
+      <c r="C50" s="208"/>
+      <c r="D50" s="209"/>
       <c r="E50" s="142">
         <f>SUM(E49)</f>
         <v>20000</v>
@@ -25026,8 +25039,8 @@
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
-      <c r="H50" s="206"/>
-      <c r="I50" s="207"/>
+      <c r="H50" s="208"/>
+      <c r="I50" s="209"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B52" s="33" t="s">
@@ -25823,8 +25836,8 @@
       <c r="D44" s="74" t="s">
         <v>338</v>
       </c>
-      <c r="E44" s="206"/>
-      <c r="F44" s="207"/>
+      <c r="E44" s="208"/>
+      <c r="F44" s="209"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B45" s="79">

</xml_diff>

<commit_message>
LP - work in progress
</commit_message>
<xml_diff>
--- a/specifications/lp/Business intelligence systems - Project - Loan Portfolio Data Specification - V6.5.xlsx
+++ b/specifications/lp/Business intelligence systems - Project - Loan Portfolio Data Specification - V6.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ShrForms\specifications\lp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941AF8CC-3377-4910-BD89-CCFEC014F8C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431FC3DB-BE48-4B2A-87A1-1C0D0C0C65A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="804" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2659" uniqueCount="1646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2661" uniqueCount="1650">
   <si>
     <t>Field ID</t>
   </si>
@@ -5340,9 +5340,6 @@
     <t>Choice(loan_purpose.csv,4)</t>
   </si>
   <si>
-    <t>Choice(repayment_terms.csv,6)</t>
-  </si>
-  <si>
     <t>Choice(reference_interest_rate.csv,3)</t>
   </si>
   <si>
@@ -5380,6 +5377,21 @@
   </si>
   <si>
     <t>Choice(covenant_type.csv,3)</t>
+  </si>
+  <si>
+    <t>Choice(igf_purpose.csv,4)</t>
+  </si>
+  <si>
+    <t>Choice(igf_security_type.csv,3)</t>
+  </si>
+  <si>
+    <t>Choice(repayment_terms.csv,4)</t>
+  </si>
+  <si>
+    <t>If Reference Interest Rate = 'Interest free' then must = 'Waived'</t>
+  </si>
+  <si>
+    <t>16(iv). Date of valuation must fall within default date range based on Date of Return (50 years)</t>
   </si>
 </sst>
 </file>
@@ -6561,19 +6573,19 @@
     <xf numFmtId="0" fontId="32" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9290,12 +9302,12 @@
       <c r="D8" s="217" t="s">
         <v>173</v>
       </c>
-      <c r="E8" s="218"/>
-      <c r="F8" s="219"/>
+      <c r="E8" s="220"/>
+      <c r="F8" s="218"/>
       <c r="G8" s="217" t="s">
         <v>174</v>
       </c>
-      <c r="H8" s="219"/>
+      <c r="H8" s="218"/>
       <c r="I8" s="74"/>
       <c r="J8" s="74"/>
     </row>
@@ -9303,15 +9315,15 @@
       <c r="C9" s="75">
         <v>1431</v>
       </c>
-      <c r="D9" s="220" t="s">
+      <c r="D9" s="221" t="s">
         <v>448</v>
       </c>
-      <c r="E9" s="220"/>
-      <c r="F9" s="220"/>
-      <c r="G9" s="222">
+      <c r="E9" s="221"/>
+      <c r="F9" s="221"/>
+      <c r="G9" s="219">
         <v>1000.1</v>
       </c>
-      <c r="H9" s="222"/>
+      <c r="H9" s="219"/>
       <c r="I9" s="78" t="s">
         <v>1121</v>
       </c>
@@ -9323,15 +9335,15 @@
       <c r="C10" s="75">
         <v>1432</v>
       </c>
-      <c r="D10" s="220" t="s">
+      <c r="D10" s="221" t="s">
         <v>457</v>
       </c>
-      <c r="E10" s="220"/>
-      <c r="F10" s="220"/>
-      <c r="G10" s="222">
+      <c r="E10" s="221"/>
+      <c r="F10" s="221"/>
+      <c r="G10" s="219">
         <v>2000.9</v>
       </c>
-      <c r="H10" s="222"/>
+      <c r="H10" s="219"/>
       <c r="I10" s="78" t="s">
         <v>1121</v>
       </c>
@@ -9356,12 +9368,12 @@
       <c r="D12" s="217" t="s">
         <v>336</v>
       </c>
-      <c r="E12" s="219"/>
+      <c r="E12" s="218"/>
       <c r="F12" s="217" t="s">
         <v>338</v>
       </c>
-      <c r="G12" s="218"/>
-      <c r="H12" s="219"/>
+      <c r="G12" s="220"/>
+      <c r="H12" s="218"/>
       <c r="I12" s="74"/>
       <c r="J12" s="74"/>
     </row>
@@ -9369,15 +9381,15 @@
       <c r="C13" s="75">
         <v>13475</v>
       </c>
-      <c r="D13" s="220" t="s">
+      <c r="D13" s="221" t="s">
         <v>899</v>
       </c>
-      <c r="E13" s="220"/>
-      <c r="F13" s="220" t="s">
+      <c r="E13" s="221"/>
+      <c r="F13" s="221" t="s">
         <v>878</v>
       </c>
-      <c r="G13" s="220"/>
-      <c r="H13" s="220"/>
+      <c r="G13" s="221"/>
+      <c r="H13" s="221"/>
       <c r="I13" s="78" t="s">
         <v>1121</v>
       </c>
@@ -9389,15 +9401,15 @@
       <c r="C14" s="75">
         <v>13476</v>
       </c>
-      <c r="D14" s="220" t="s">
+      <c r="D14" s="221" t="s">
         <v>917</v>
       </c>
-      <c r="E14" s="220"/>
-      <c r="F14" s="220" t="s">
+      <c r="E14" s="221"/>
+      <c r="F14" s="221" t="s">
         <v>880</v>
       </c>
-      <c r="G14" s="220"/>
-      <c r="H14" s="220"/>
+      <c r="G14" s="221"/>
+      <c r="H14" s="221"/>
       <c r="I14" s="78" t="s">
         <v>1121</v>
       </c>
@@ -9607,8 +9619,8 @@
       <c r="E25" s="217" t="s">
         <v>332</v>
       </c>
-      <c r="F25" s="218"/>
-      <c r="G25" s="219"/>
+      <c r="F25" s="220"/>
+      <c r="G25" s="218"/>
       <c r="H25" s="74" t="s">
         <v>1123</v>
       </c>
@@ -9668,12 +9680,12 @@
       <c r="D29" s="217" t="s">
         <v>336</v>
       </c>
-      <c r="E29" s="219"/>
+      <c r="E29" s="218"/>
       <c r="F29" s="217" t="s">
         <v>338</v>
       </c>
-      <c r="G29" s="218"/>
-      <c r="H29" s="219"/>
+      <c r="G29" s="220"/>
+      <c r="H29" s="218"/>
       <c r="I29" s="80"/>
       <c r="J29" s="74"/>
     </row>
@@ -9681,15 +9693,15 @@
       <c r="C30" s="75">
         <v>13473</v>
       </c>
-      <c r="D30" s="220" t="s">
+      <c r="D30" s="221" t="s">
         <v>899</v>
       </c>
-      <c r="E30" s="220"/>
-      <c r="F30" s="220" t="s">
+      <c r="E30" s="221"/>
+      <c r="F30" s="221" t="s">
         <v>878</v>
       </c>
-      <c r="G30" s="220"/>
-      <c r="H30" s="220"/>
+      <c r="G30" s="221"/>
+      <c r="H30" s="221"/>
       <c r="I30" s="78" t="s">
         <v>1121</v>
       </c>
@@ -9701,15 +9713,15 @@
       <c r="C31" s="75">
         <v>13474</v>
       </c>
-      <c r="D31" s="220" t="s">
+      <c r="D31" s="221" t="s">
         <v>921</v>
       </c>
-      <c r="E31" s="220"/>
-      <c r="F31" s="220" t="s">
+      <c r="E31" s="221"/>
+      <c r="F31" s="221" t="s">
         <v>880</v>
       </c>
-      <c r="G31" s="220"/>
-      <c r="H31" s="220"/>
+      <c r="G31" s="221"/>
+      <c r="H31" s="221"/>
       <c r="I31" s="78" t="s">
         <v>1121</v>
       </c>
@@ -9728,11 +9740,11 @@
       <c r="D33" s="217" t="s">
         <v>356</v>
       </c>
-      <c r="E33" s="219"/>
+      <c r="E33" s="218"/>
       <c r="F33" s="217" t="s">
         <v>171</v>
       </c>
-      <c r="G33" s="219"/>
+      <c r="G33" s="218"/>
       <c r="H33" s="81" t="s">
         <v>172</v>
       </c>
@@ -9743,14 +9755,14 @@
       <c r="C34" s="75">
         <v>1454</v>
       </c>
-      <c r="D34" s="220" t="s">
+      <c r="D34" s="221" t="s">
         <v>1140</v>
       </c>
-      <c r="E34" s="220"/>
-      <c r="F34" s="221">
+      <c r="E34" s="221"/>
+      <c r="F34" s="222">
         <v>43133</v>
       </c>
-      <c r="G34" s="221"/>
+      <c r="G34" s="222"/>
       <c r="H34" s="84">
         <v>43134</v>
       </c>
@@ -9765,14 +9777,14 @@
       <c r="C35" s="75">
         <v>1455</v>
       </c>
-      <c r="D35" s="220" t="s">
+      <c r="D35" s="221" t="s">
         <v>1140</v>
       </c>
-      <c r="E35" s="220"/>
-      <c r="F35" s="221">
+      <c r="E35" s="221"/>
+      <c r="F35" s="222">
         <v>43132</v>
       </c>
-      <c r="G35" s="221"/>
+      <c r="G35" s="222"/>
       <c r="H35" s="84">
         <v>43159</v>
       </c>
@@ -9788,24 +9800,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="D33:E33"/>
     <mergeCell ref="E25:G25"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="F30:H30"/>
@@ -9813,6 +9807,24 @@
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15381,8 +15393,8 @@
   <dimension ref="A1:AA208"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M79" sqref="M79"/>
+      <pane ySplit="8" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16635,7 +16647,7 @@
         <v>188</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>1294</v>
+        <v>1645</v>
       </c>
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
@@ -16970,7 +16982,7 @@
         <v>193</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>1295</v>
+        <v>1646</v>
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="17"/>
@@ -17165,7 +17177,7 @@
         <v>1280</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>1331</v>
+        <v>1630</v>
       </c>
       <c r="F44" s="17"/>
       <c r="G44" s="17"/>
@@ -17263,7 +17275,7 @@
         <v>1282</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>1296</v>
+        <v>1647</v>
       </c>
       <c r="F46" s="17"/>
       <c r="G46" s="17"/>
@@ -17312,7 +17324,7 @@
         <v>1283</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>1297</v>
+        <v>1632</v>
       </c>
       <c r="F47" s="17"/>
       <c r="G47" s="17"/>
@@ -17468,7 +17480,10 @@
         <v>129</v>
       </c>
       <c r="L50" s="10"/>
-      <c r="M50" s="101"/>
+      <c r="M50" s="115" t="b">
+        <f>H50</f>
+        <v>1</v>
+      </c>
       <c r="N50" s="10" t="s">
         <v>1459</v>
       </c>
@@ -19067,7 +19082,7 @@
         <v>173</v>
       </c>
       <c r="E84" s="23" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="F84" s="17"/>
       <c r="G84" s="17"/>
@@ -19254,7 +19269,7 @@
         <v>176</v>
       </c>
       <c r="E88" s="23" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="F88" s="17"/>
       <c r="G88" s="17"/>
@@ -19674,7 +19689,7 @@
         <v>182</v>
       </c>
       <c r="E97" s="23" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="F97" s="17"/>
       <c r="G97" s="17"/>
@@ -19928,7 +19943,7 @@
         <v>336</v>
       </c>
       <c r="E103" s="23" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="F103" s="17"/>
       <c r="G103" s="17"/>
@@ -20375,7 +20390,7 @@
     </row>
     <row r="113" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="B113" s="23" t="s">
         <v>21</v>
@@ -20815,7 +20830,7 @@
         <v>1</v>
       </c>
       <c r="P121" s="94" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="Q121" s="101"/>
       <c r="R121" s="10"/>
@@ -20940,7 +20955,7 @@
         <v>404</v>
       </c>
       <c r="E124" s="23" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="F124" s="17"/>
       <c r="G124" s="17"/>
@@ -21266,7 +21281,7 @@
         <v>1377</v>
       </c>
       <c r="E131" s="178" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="F131" s="17"/>
       <c r="G131" s="17"/>
@@ -21494,7 +21509,7 @@
         <v>0</v>
       </c>
       <c r="P136" s="10" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="Q136" s="101"/>
       <c r="R136" s="10"/>
@@ -21833,7 +21848,7 @@
         <v>166</v>
       </c>
       <c r="E143" s="23" t="s">
-        <v>1632</v>
+        <v>1647</v>
       </c>
       <c r="F143" s="17"/>
       <c r="G143" s="17"/>
@@ -21879,7 +21894,7 @@
         <v>167</v>
       </c>
       <c r="E144" s="23" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="F144" s="17"/>
       <c r="G144" s="17"/>
@@ -22060,7 +22075,10 @@
         <v>129</v>
       </c>
       <c r="L147" s="10"/>
-      <c r="M147" s="101"/>
+      <c r="M147" s="115" t="b">
+        <f>IF(H146&lt;3.5,H147,TRUE)</f>
+        <v>1</v>
+      </c>
       <c r="N147" s="10" t="s">
         <v>1461</v>
       </c>
@@ -22072,10 +22090,7 @@
       <c r="T147" s="10"/>
       <c r="U147" s="101"/>
       <c r="V147" s="10"/>
-      <c r="W147" s="118" t="b">
-        <f>OR(H145&gt;20,H146&lt;3.5)</f>
-        <v>0</v>
-      </c>
+      <c r="W147" s="118"/>
       <c r="X147" s="10"/>
       <c r="Y147" s="16" t="s">
         <v>381</v>
@@ -22232,7 +22247,7 @@
         <v>1</v>
       </c>
       <c r="P150" s="10" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="Q150" s="101"/>
       <c r="R150" s="10"/>
@@ -22431,8 +22446,13 @@
       <c r="L154" s="10" t="s">
         <v>1261</v>
       </c>
-      <c r="M154" s="101"/>
-      <c r="N154" s="10"/>
+      <c r="M154" s="101" t="b">
+        <f>IF(H144=4, H154=4,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="N154" s="10" t="s">
+        <v>1648</v>
+      </c>
       <c r="O154" s="101"/>
       <c r="P154" s="10"/>
       <c r="Q154" s="101"/>
@@ -22809,8 +22829,13 @@
       <c r="N162" s="10" t="s">
         <v>1481</v>
       </c>
-      <c r="O162" s="122"/>
-      <c r="P162" s="10"/>
+      <c r="O162" s="122" t="b">
+        <f>AND(H162&gt;=H206,H162&lt;=H207)</f>
+        <v>1</v>
+      </c>
+      <c r="P162" s="10" t="s">
+        <v>1649</v>
+      </c>
       <c r="Q162" s="101"/>
       <c r="R162" s="10"/>
       <c r="S162" s="101"/>
@@ -22841,7 +22866,7 @@
         <v>1000</v>
       </c>
       <c r="E163" s="178" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="F163" s="17"/>
       <c r="G163" s="17"/>
@@ -23516,7 +23541,7 @@
         <v>1</v>
       </c>
       <c r="N178" s="10" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="O178" s="101"/>
       <c r="P178" s="10"/>
@@ -23655,7 +23680,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="10" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="O181" s="101"/>
       <c r="P181" s="10"/>

</xml_diff>